<commit_message>
Small Comment to maintain contribution streak
</commit_message>
<xml_diff>
--- a/Final Predictions.xlsx
+++ b/Final Predictions.xlsx
@@ -778,7 +778,7 @@
         <v>933</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1010,7 +1010,7 @@
         <v>962</v>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1082,7 +1082,7 @@
         <v>971</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1498,7 +1498,7 @@
         <v>1023</v>
       </c>
       <c r="B133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -1634,7 +1634,7 @@
         <v>1040</v>
       </c>
       <c r="B150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -3514,7 +3514,7 @@
         <v>1275</v>
       </c>
       <c r="B385" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386">
@@ -3562,7 +3562,7 @@
         <v>1281</v>
       </c>
       <c r="B391" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392">

</xml_diff>